<commit_message>
Updated Behaviour Matrix Updated full learning mode Updated x-y-altitude selective learning as per the updates on behaviour matrix (flight modes matrix)
</commit_message>
<xml_diff>
--- a/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
+++ b/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="39">
   <si>
     <t xml:space="preserve">RC Stabilize</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Full Learning Automated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning Selective X/Y/Altitude</t>
   </si>
   <si>
     <t xml:space="preserve">Leaf Mission</t>
@@ -140,6 +143,9 @@
   </si>
   <si>
     <t xml:space="preserve">CTW estimation from pilot command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTW estimation from pilot throttle command</t>
   </si>
 </sst>
 </file>
@@ -365,13 +371,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.38"/>
@@ -382,8 +388,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,340 +415,375 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" s="6"/>
+      <c r="J3" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="34.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="34.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="9"/>
@@ -753,6 +795,7 @@
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="9"/>
@@ -764,109 +807,122 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="55.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="55.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="55.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,30 +935,48 @@
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="J25" s="4" t="s">
-        <v>9</v>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed CTW estimation to RC Stabilize - Hover Thrust Identification mode. Changed Full Learning mode name in behaviour matrix
</commit_message>
<xml_diff>
--- a/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
+++ b/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">X/Y/Altitude Learning </t>
   </si>
   <si>
-    <t xml:space="preserve">Full Learning Automated</t>
+    <t xml:space="preserve">Full Learning</t>
   </si>
   <si>
     <t xml:space="preserve">Learning Selective X/Y/Altitude</t>
@@ -420,11 +420,11 @@
   </sheetPr>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.38"/>

</xml_diff>

<commit_message>
Updated Behaviour Matrix with latest timestamp
</commit_message>
<xml_diff>
--- a/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
+++ b/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
@@ -333,12 +333,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -420,8 +420,8 @@
   </sheetPr>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G22" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -876,7 +876,7 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -889,7 +889,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -900,7 +900,7 @@
       <c r="A18" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -930,7 +930,7 @@
       <c r="A19" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -960,7 +960,7 @@
       <c r="A20" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -990,7 +990,7 @@
       <c r="A21" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -1022,7 +1022,7 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -1036,7 +1036,7 @@
       <c r="D23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="13"/>
+      <c r="G23" s="14"/>
       <c r="H23" s="6" t="s">
         <v>11</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="B24" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="13"/>
+      <c r="G24" s="14"/>
       <c r="H24" s="6" t="s">
         <v>11</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="F25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="13"/>
+      <c r="G25" s="14"/>
       <c r="H25" s="6" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1088,7 @@
       <c r="L25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="12"/>
@@ -1114,7 +1114,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="12"/>

</xml_diff>

<commit_message>
fixes to FSAC behaviour
</commit_message>
<xml_diff>
--- a/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
+++ b/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="46">
   <si>
     <t xml:space="preserve">RC Stabilize</t>
   </si>
@@ -123,6 +123,10 @@
 steady state, use current 
 Tuning, and update the new 
 tuning in cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">✓
+Once Steady-State detected → exist MRFT oscillations</t>
   </si>
   <si>
     <t xml:space="preserve">E3</t>
@@ -171,7 +175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -201,12 +205,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -277,7 +275,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -316,10 +314,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -417,8 +411,8 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O19" activeCellId="0" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -728,7 +722,7 @@
       <c r="I10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="5" t="s">
@@ -736,7 +730,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="5"/>
@@ -754,7 +748,7 @@
       <c r="I11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="5"/>
@@ -785,7 +779,7 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -808,7 +802,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -843,7 +837,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="5"/>
@@ -872,36 +866,36 @@
       <c r="L15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -927,11 +921,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -951,18 +945,18 @@
         <v>11</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="55.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="13" t="s">
         <v>34</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>11</v>
@@ -981,33 +975,33 @@
         <v>11</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="14"/>
+      <c r="G22" s="13"/>
       <c r="H22" s="6" t="s">
         <v>11</v>
       </c>
@@ -1026,9 +1020,9 @@
     </row>
     <row r="23" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="14"/>
+        <v>37</v>
+      </c>
+      <c r="G23" s="13"/>
       <c r="H23" s="6" t="s">
         <v>11</v>
       </c>
@@ -1042,12 +1036,12 @@
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="14"/>
+      <c r="G24" s="13"/>
       <c r="H24" s="6" t="s">
         <v>11</v>
       </c>
@@ -1059,23 +1053,23 @@
       <c r="L24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
+      <c r="B25" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>11</v>
@@ -1085,23 +1079,23 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
+      <c r="B27" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E28" s="5"/>
       <c r="K28" s="5" t="s">
@@ -1110,7 +1104,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>11</v>
@@ -1122,7 +1116,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>11</v>
@@ -1130,7 +1124,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J44" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
formatted  Behaviour Matrix.xlsx to improve readability
</commit_message>
<xml_diff>
--- a/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
+++ b/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="46">
   <si>
     <t xml:space="preserve">RC Stabilize</t>
   </si>
@@ -175,7 +175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -200,14 +200,53 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,8 +255,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAD8"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFA6"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFAFAD8"/>
       </patternFill>
     </fill>
     <fill>
@@ -226,20 +271,19 @@
         <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFAFAD8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -275,11 +319,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,47 +336,87 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,7 +449,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFAFAD8"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -409,58 +497,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1048576"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O19" activeCellId="0" sqref="O19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="H24 J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="41.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.04"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="1" t="s">
+    <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -501,7 +591,7 @@
       <c r="O2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -512,30 +602,31 @@
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="0" t="s">
+      <c r="L3" s="1"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -578,12 +669,12 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="6" t="s">
         <v>11</v>
       </c>
@@ -607,16 +698,16 @@
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="6" t="s">
         <v>11</v>
       </c>
@@ -634,23 +725,23 @@
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="5" t="s">
         <v>11</v>
       </c>
@@ -659,8 +750,8 @@
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
@@ -682,22 +773,24 @@
       <c r="K8" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="L8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="35.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="5"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="L9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="34.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
@@ -706,8 +799,8 @@
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -716,42 +809,43 @@
       <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="17" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="L10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="5"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="5" t="s">
         <v>11</v>
       </c>
@@ -760,49 +854,52 @@
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="9" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="5"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="18" t="s">
         <v>27</v>
       </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="1"/>
       <c r="G13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="5"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="18" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -837,11 +934,11 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="5" t="s">
         <v>11</v>
       </c>
@@ -863,45 +960,49 @@
       <c r="K15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="5"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+    </row>
+    <row r="18" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="6" t="s">
         <v>11</v>
       </c>
@@ -921,17 +1022,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="6" t="s">
         <v>11</v>
       </c>
@@ -944,24 +1047,26 @@
       <c r="J19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="11" t="s">
         <v>33</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="6" t="s">
         <v>11</v>
       </c>
@@ -974,7 +1079,7 @@
       <c r="J20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="11" t="s">
         <v>33</v>
       </c>
       <c r="L20" s="5" t="s">
@@ -982,152 +1087,241 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+    </row>
+    <row r="23" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="22"/>
+      <c r="H25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="L25" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+    </row>
+    <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="13" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="K29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+    </row>
+    <row r="31" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="K28" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J44" s="0" t="s">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J47" s="0" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added refined tuning - collect data mission mode to excel behaviour matrix
</commit_message>
<xml_diff>
--- a/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
+++ b/Guide/HEAR Software/Flight Modes/Behaviour Matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="47">
   <si>
     <t xml:space="preserve">RC Stabilize</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Leaf Mission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refined Tuning – Collect Data</t>
   </si>
   <si>
     <t xml:space="preserve">RC Available</t>
@@ -499,8 +502,8 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="H24 J24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N34" activeCellId="0" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -511,13 +514,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="41.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.04"/>
   </cols>
   <sheetData>
@@ -553,231 +556,251 @@
       <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
       <c r="O3" s="12"/>
       <c r="P3" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="9"/>
       <c r="G5" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="9"/>
       <c r="G6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="9"/>
       <c r="G7" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="35.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="11"/>
@@ -788,179 +811,200 @@
       <c r="I9" s="14"/>
       <c r="J9" s="11"/>
       <c r="K9" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="34.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L10" s="1"/>
+      <c r="M10" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="34.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="1"/>
+      <c r="M12" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L15" s="11"/>
+      <c r="M15" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
@@ -975,6 +1019,7 @@
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
@@ -989,102 +1034,108 @@
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="53.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="53.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="M20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19"/>
@@ -1099,6 +1150,7 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
@@ -1113,37 +1165,39 @@
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="22"/>
       <c r="H23" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="M23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1151,41 +1205,43 @@
       <c r="F24" s="1"/>
       <c r="G24" s="22"/>
       <c r="H24" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="11"/>
+      <c r="M24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="20"/>
@@ -1197,9 +1253,8 @@
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
       <c r="K26" s="20"/>
-      <c r="L26" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="19"/>
@@ -1214,10 +1269,11 @@
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
@@ -1229,10 +1285,11 @@
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
+      <c r="M28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1241,17 +1298,18 @@
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
       <c r="I29" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
@@ -1263,10 +1321,11 @@
       <c r="J30" s="24"/>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
+      <c r="M30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1277,38 +1336,40 @@
       <c r="I31" s="22"/>
       <c r="J31" s="1"/>
       <c r="K31" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
       <c r="I32" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="11"/>
       <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
@@ -1316,10 +1377,11 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J47" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>